<commit_message>
commit chaos feature work so far and commit new files for tracking
</commit_message>
<xml_diff>
--- a/Chaotic_features.xlsx
+++ b/Chaotic_features.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psturge\Google Drive\RuneQuest\RQG\GM_aids\Stat_blocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psturge.WARWICK\My Drive\RuneQuest\RQG\GM_aids\Stat_blocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2C6243-34B0-4198-AF59-C96EDE2E29BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="12105"/>
+    <workbookView xWindow="7485" yWindow="4695" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Curse of Thed" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="140">
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
   <si>
     <t>+1D6 POW</t>
   </si>
@@ -35,12 +43,12 @@
     <t>+3D6 POW</t>
   </si>
   <si>
+    <t>+2D6 DEX</t>
+  </si>
+  <si>
     <t>+4D6 DEX</t>
   </si>
   <si>
-    <t>+2D6 DEX</t>
-  </si>
-  <si>
     <t>+2D6 STR</t>
   </si>
   <si>
@@ -53,6 +61,9 @@
     <t>+4D6 CON</t>
   </si>
   <si>
+    <t>+2D6 SIZ</t>
+  </si>
+  <si>
     <t>+4D6 SIZ</t>
   </si>
   <si>
@@ -158,19 +169,289 @@
     <t>Roll from the Curse of Thed table on page 95.</t>
   </si>
   <si>
-    <t>Roll</t>
-  </si>
-  <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>+2D6 SIZ</t>
+    <t>01–03</t>
+  </si>
+  <si>
+    <t>Lose 1D6 POW</t>
+  </si>
+  <si>
+    <t>04–05</t>
+  </si>
+  <si>
+    <t>Lose 2D6 POW</t>
+  </si>
+  <si>
+    <t>Lose 3D6 POW</t>
+  </si>
+  <si>
+    <t>07–09</t>
+  </si>
+  <si>
+    <t>Lose 1D6 DEX</t>
+  </si>
+  <si>
+    <t>10–11</t>
+  </si>
+  <si>
+    <t>Lose 2D6 DEX</t>
+  </si>
+  <si>
+    <t>Lose 3D6 DEX</t>
+  </si>
+  <si>
+    <t>13–14</t>
+  </si>
+  <si>
+    <t>Lose 2D6 STR</t>
+  </si>
+  <si>
+    <t>Lose 4D6 STR</t>
+  </si>
+  <si>
+    <t>16–17</t>
+  </si>
+  <si>
+    <t>Lose 2D6 CON</t>
+  </si>
+  <si>
+    <t>Lose 4D6 CON</t>
+  </si>
+  <si>
+    <t>19–20</t>
+  </si>
+  <si>
+    <t>+3 - victim’s strike rank for duration of spell.</t>
+  </si>
+  <si>
+    <t>21–22</t>
+  </si>
+  <si>
+    <t>May not resist any 1-point spells cast at the victim.</t>
+  </si>
+  <si>
+    <t>23–24</t>
+  </si>
+  <si>
+    <t>Drenched in acid, 2D10 potency (one round only).</t>
+  </si>
+  <si>
+    <t>25–26</t>
+  </si>
+  <si>
+    <t>Engulfed in flame, 3D10 damage (one round only).</t>
+  </si>
+  <si>
+    <t>27–28</t>
+  </si>
+  <si>
+    <t>Attracts magic: all 1-point attack spells cast in a 20-meter radius automatically targets against the victim.</t>
+  </si>
+  <si>
+    <t>29–30</t>
+  </si>
+  <si>
+    <t>Victim becomes immune - fire damage for duration of spell.</t>
+  </si>
+  <si>
+    <t>31–32</t>
+  </si>
+  <si>
+    <t>Roll equal - or below INT×5 on D100 or stand stupefied for 15 minutes.</t>
+  </si>
+  <si>
+    <t>33–35</t>
+  </si>
+  <si>
+    <t>All foes have +20% chance - hit victim*.</t>
+  </si>
+  <si>
+    <t>36–37</t>
+  </si>
+  <si>
+    <t>One valuable gem, magic item, or weapon in the victim’s possession is eaten by Chaos and disappears forever.</t>
+  </si>
+  <si>
+    <t>38–40</t>
+  </si>
+  <si>
+    <t>Takes 1 point of damage in random location each melee round until spell expires*.</t>
+  </si>
+  <si>
+    <t>41–42</t>
+  </si>
+  <si>
+    <t>Victim befuddled for spell duration.</t>
+  </si>
+  <si>
+    <t>43–45</t>
+  </si>
+  <si>
+    <t>Non-Rune metals do double damage - victim.</t>
+  </si>
+  <si>
+    <t>Victim is rendered incapable of physically attacking*.</t>
+  </si>
+  <si>
+    <t>47–48</t>
+  </si>
+  <si>
+    <t>All foes have +30% chance - hit victim*.</t>
+  </si>
+  <si>
+    <t>49–50</t>
+  </si>
+  <si>
+    <t>Attacked by poison, 2D10 potency (one round only).</t>
+  </si>
+  <si>
+    <t>51–52</t>
+  </si>
+  <si>
+    <t>Takes 3 points of damage in random location each melee round until spell expires*.</t>
+  </si>
+  <si>
+    <t>53–54</t>
+  </si>
+  <si>
+    <t>Add +3 - damage of all weapons hitting the victim*.</t>
+  </si>
+  <si>
+    <t>55–56</t>
+  </si>
+  <si>
+    <t>Victim bound as in Slow spell.</t>
+  </si>
+  <si>
+    <t>57–58</t>
+  </si>
+  <si>
+    <t>Victim may not resist 1- or 2-point spells.</t>
+  </si>
+  <si>
+    <t>59–60</t>
+  </si>
+  <si>
+    <t>A spirit of 3D6 POW engages in spirit combat with the victim.</t>
+  </si>
+  <si>
+    <t>61–62</t>
+  </si>
+  <si>
+    <t>Explosion, 3D6 damage - all within 3 meters, as well as - victim (one round only).</t>
+  </si>
+  <si>
+    <t>63–65</t>
+  </si>
+  <si>
+    <t>Victim becomes physically indistinguishable from caster of spell.</t>
+  </si>
+  <si>
+    <t>66–67</t>
+  </si>
+  <si>
+    <t>Victim becomes silent when moving; adds +25% permanently - Move Silent ability.</t>
+  </si>
+  <si>
+    <t>68–70</t>
+  </si>
+  <si>
+    <t>Target becomes magic attractant for 1- and 2-point spells: all spirit magic spells cast at anyone, beneficial or harmful,</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>within 3 meters of the target instead strike target.</t>
+  </si>
+  <si>
+    <t>71–72</t>
+  </si>
+  <si>
+    <t>Add +4 points - all weapon damage against the victim*.</t>
+  </si>
+  <si>
+    <t>73–74</t>
+  </si>
+  <si>
+    <t>As above but add +5 points*.</t>
+  </si>
+  <si>
+    <t>75–76</t>
+  </si>
+  <si>
+    <t>As above but add +6 points*.</t>
+  </si>
+  <si>
+    <t>Victim may use no offensive magic*.</t>
+  </si>
+  <si>
+    <t>78–80</t>
+  </si>
+  <si>
+    <t>Victim takes 10D6 points of damage in random location each round until spell expires*.</t>
+  </si>
+  <si>
+    <t>81–82</t>
+  </si>
+  <si>
+    <t>Victim immobilized.</t>
+  </si>
+  <si>
+    <t>83–84</t>
+  </si>
+  <si>
+    <t>Victim goes berserk as in Fanaticism spell.</t>
+  </si>
+  <si>
+    <t>Foes have +40% chance - hit victim.</t>
+  </si>
+  <si>
+    <t>86–87</t>
+  </si>
+  <si>
+    <t>All objects on victim’s body are devoured by Chaos, and victim stands naked and weaponless.</t>
+  </si>
+  <si>
+    <t>88–90</t>
+  </si>
+  <si>
+    <t>Victim may make no vocal sounds, including spell casting.</t>
+  </si>
+  <si>
+    <t>91–92</t>
+  </si>
+  <si>
+    <t>Roll CON×5 or lose consciousness for spell duration.</t>
+  </si>
+  <si>
+    <t>93–94</t>
+  </si>
+  <si>
+    <t>Victim becomes magic attractant for all spells (see entry 68-70).</t>
+  </si>
+  <si>
+    <t>95–96</t>
+  </si>
+  <si>
+    <t>Victim Demoralized for spell duration as per spell.</t>
+  </si>
+  <si>
+    <t>97–98</t>
+  </si>
+  <si>
+    <t>Lose 2D6 SIZ.</t>
+  </si>
+  <si>
+    <t>Roll twice, rolling again if this result is rolled once more.</t>
+  </si>
+  <si>
+    <t>Victim joins caster’s side for duration of spell.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -202,15 +483,21 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -221,6 +508,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="CurseOfThed" displayName="CurseOfThed" ref="A1:B52">
+  <autoFilter ref="A1:B52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Roll" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Feature"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -485,10 +783,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -499,10 +797,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -510,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -518,7 +816,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -526,7 +824,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -534,7 +832,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -542,7 +840,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -550,31 +848,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>4</v>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -582,7 +880,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -590,7 +888,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -598,7 +896,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -606,7 +904,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -614,7 +912,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -622,31 +920,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>46</v>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>46</v>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>9</v>
+      <c r="B19" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -654,7 +952,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -662,7 +960,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -670,7 +968,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -678,7 +976,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -686,7 +984,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -694,7 +992,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -702,7 +1000,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -710,7 +1008,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -718,7 +1016,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -726,7 +1024,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -734,7 +1032,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -742,23 +1040,23 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -766,7 +1064,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +1072,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -782,7 +1080,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +1088,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,7 +1096,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -806,7 +1104,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -814,7 +1112,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,7 +1120,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -830,7 +1128,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -838,7 +1136,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -846,7 +1144,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -854,7 +1152,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -862,7 +1160,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -870,7 +1168,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -878,7 +1176,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -886,7 +1184,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -894,7 +1192,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -902,7 +1200,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -910,7 +1208,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -918,7 +1216,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -926,7 +1224,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -934,7 +1232,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -942,7 +1240,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -950,7 +1248,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -958,7 +1256,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -966,7 +1264,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -974,7 +1272,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -982,7 +1280,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -990,7 +1288,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -998,7 +1296,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1006,7 +1304,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1014,7 +1312,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1022,7 +1320,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1030,7 +1328,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1038,7 +1336,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1046,7 +1344,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1054,7 +1352,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1062,7 +1360,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1070,7 +1368,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1078,7 +1376,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1086,7 +1384,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1094,7 +1392,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1102,7 +1400,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1110,7 +1408,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1118,7 +1416,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1126,7 +1424,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1134,7 +1432,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1142,7 +1440,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1150,7 +1448,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1158,7 +1456,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1166,7 +1464,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1174,7 +1472,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1182,7 +1480,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1190,7 +1488,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1198,7 +1496,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1206,7 +1504,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1214,7 +1512,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1222,7 +1520,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1230,7 +1528,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1238,7 +1536,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1246,7 +1544,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1254,7 +1552,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1262,7 +1560,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1270,7 +1568,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1278,7 +1576,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1286,7 +1584,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1294,7 +1592,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1302,11 +1600,448 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>85</v>
+      </c>
+      <c r="B44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B49" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>99</v>
+      </c>
+      <c r="B51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>